<commit_message>
fix hand size glitch
</commit_message>
<xml_diff>
--- a/table of levels.xlsx
+++ b/table of levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valky\AppData\Roaming\Balatro\Mods\upgrademod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A2FEAD-FC35-4EF6-B68C-B3C9F17E000B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CBAE6-508D-44A9-BB86-56FAE39CFEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="11" xr2:uid="{61FB6368-C9E5-4A96-AA5B-F7BF30B3F17F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{61FB6368-C9E5-4A96-AA5B-F7BF30B3F17F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mult" sheetId="2" r:id="rId1"/>
@@ -6456,7 +6456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96240DC4-48F2-4250-90A0-94515EDF05F3}">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -11270,8 +11270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B788F6-59A9-44CE-B687-94279AF0D375}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>

</xml_diff>